<commit_message>
Connected Report and Powerpoints with out clustering co efficient
</commit_message>
<xml_diff>
--- a/ComplexNetwork1/src/result/US_CA.xlsx
+++ b/ComplexNetwork1/src/result/US_CA.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="connected component" sheetId="3" r:id="rId1"/>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -322,8 +322,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,44 +625,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861E1950-09F6-4D9A-A830-55218BC12E9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -645,20 +673,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -666,7 +693,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -674,7 +701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -682,7 +709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -690,7 +717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -698,7 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -706,7 +733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -714,7 +741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -722,7 +749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -730,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -738,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -746,7 +773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -754,7 +781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -762,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -770,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -778,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -786,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -794,7 +821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -802,7 +829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -810,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -818,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -826,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -834,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -842,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -850,7 +877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -858,7 +885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -866,7 +893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -874,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -882,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -890,7 +917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -898,7 +925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -906,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -914,7 +941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -922,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -930,7 +957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -938,7 +965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -946,7 +973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -954,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -962,7 +989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -970,7 +997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -978,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -986,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -994,7 +1021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1002,7 +1029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -1010,7 +1037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -1018,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -1026,7 +1053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1034,7 +1061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1042,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1066,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -1074,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1090,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -1098,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -1106,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1114,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -1122,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>27</v>
       </c>
@@ -1130,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>28</v>
       </c>
@@ -1138,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -1146,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -1154,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -1162,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -1170,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -1178,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>41</v>
       </c>
@@ -1186,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -1194,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>46</v>
       </c>
@@ -1202,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -1210,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -1218,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>49</v>
       </c>
@@ -1226,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>53</v>
       </c>
@@ -1234,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>54</v>
       </c>
@@ -1242,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -1250,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -1258,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>69</v>
       </c>
@@ -1266,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>72</v>
       </c>
@@ -1274,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -1282,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -1290,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -1298,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>

</xml_diff>